<commit_message>
Set up Week 3 RMD
</commit_message>
<xml_diff>
--- a/data/Data for Week 1.xlsx
+++ b/data/Data for Week 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c1412fc621fc485b/Matina/Cal Poly/2nd Year/3. Spring 2024/ECON 339/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c1412fc621fc485b/Matina/Cal Poly/2nd Year/3. Spring 2024/Econ-339/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="419" documentId="13_ncr:1_{975376BA-4F9F-487E-B760-3B4E5F779A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{881D2BB8-61D2-4E92-B0E6-4488C854650B}"/>
   <bookViews>
-    <workbookView xWindow="13815" yWindow="0" windowWidth="15090" windowHeight="15585" firstSheet="8" activeTab="8" xr2:uid="{6C626033-3C52-4C29-83C2-D43F5AB87DB7}"/>
+    <workbookView xWindow="3310" yWindow="550" windowWidth="14400" windowHeight="7530" firstSheet="8" activeTab="8" xr2:uid="{6C626033-3C52-4C29-83C2-D43F5AB87DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="CarBuyers" sheetId="15" r:id="rId1"/>

</xml_diff>